<commit_message>
[11/05/2023][2] Fixed having to os.chdir() to current folder to run Whisper -- originally for the sake of multithreading. Multithreading failed nonetheless due to some unknown error, but at least we don't have to do that wack ass s##t anymore.
</commit_message>
<xml_diff>
--- a/database/raws/Dataset.xlsx
+++ b/database/raws/Dataset.xlsx
@@ -5,16 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peter\Desktop\Fucking Around 3.0\Sheen Learning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peter\Desktop\Fucking Around 3.0\Program\database\raws\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{821D32B4-6A4A-4140-9122-B96D288DAAE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E85B9D-C708-4992-956C-E63A3865A7A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="2100" windowWidth="21600" windowHeight="13500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All of it" sheetId="1" r:id="rId1"/>
-    <sheet name="26-Feb" sheetId="2" r:id="rId2"/>
+    <sheet name="2-Jul" sheetId="4" r:id="rId2"/>
+    <sheet name="19-Feb" sheetId="2" r:id="rId3"/>
+    <sheet name="26-Feb" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="128">
   <si>
     <t>Question</t>
   </si>
@@ -220,27 +222,9 @@
     <t>R</t>
   </si>
   <si>
-    <t>Mi</t>
-  </si>
-  <si>
-    <t>Pau</t>
-  </si>
-  <si>
-    <t>Liz</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>Au</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
-    <t>An</t>
-  </si>
-  <si>
     <t>Liv</t>
   </si>
   <si>
@@ -359,6 +343,75 @@
   </si>
   <si>
     <t>St</t>
+  </si>
+  <si>
+    <t>PY</t>
+  </si>
+  <si>
+    <t>GRE</t>
+  </si>
+  <si>
+    <t>JJ</t>
+  </si>
+  <si>
+    <t>TMS</t>
+  </si>
+  <si>
+    <t>RIC</t>
+  </si>
+  <si>
+    <t>PAU</t>
+  </si>
+  <si>
+    <t>LIZ</t>
+  </si>
+  <si>
+    <t>AMD</t>
+  </si>
+  <si>
+    <t>YOR</t>
+  </si>
+  <si>
+    <t>AUD</t>
+  </si>
+  <si>
+    <t>ANT</t>
+  </si>
+  <si>
+    <t>SAM</t>
+  </si>
+  <si>
+    <t>KNC</t>
+  </si>
+  <si>
+    <t>LIV</t>
+  </si>
+  <si>
+    <t>KSMG</t>
+  </si>
+  <si>
+    <t>MAR</t>
+  </si>
+  <si>
+    <t>ENO</t>
+  </si>
+  <si>
+    <t>But do we have to step in, still? Suicide, for example. If someone kills themselves, by Sam's definition, they would have sinned unless it is prevented.</t>
+  </si>
+  <si>
+    <t>What about those who have heard of Jesus, who has already accepted him, who nonetheless committed suicide? Are they sinners still?</t>
+  </si>
+  <si>
+    <t>FIN</t>
+  </si>
+  <si>
+    <t>JER</t>
+  </si>
+  <si>
+    <t>YOT</t>
+  </si>
+  <si>
+    <t>STN</t>
   </si>
 </sst>
 </file>
@@ -679,8 +732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -715,13 +768,13 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D2" s="1">
         <v>44611</v>
       </c>
       <c r="E2" t="s">
-        <v>58</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -732,13 +785,13 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="D3" s="1">
         <v>44611</v>
       </c>
       <c r="E3" t="s">
-        <v>59</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -749,13 +802,13 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D4" s="1">
         <v>44611</v>
       </c>
       <c r="E4" t="s">
-        <v>58</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -766,13 +819,13 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D5" s="1">
         <v>44611</v>
       </c>
       <c r="E5" t="s">
-        <v>60</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -789,7 +842,7 @@
         <v>44611</v>
       </c>
       <c r="E6" t="s">
-        <v>61</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -806,7 +859,7 @@
         <v>44611</v>
       </c>
       <c r="E7" t="s">
-        <v>61</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -857,7 +910,7 @@
         <v>44611</v>
       </c>
       <c r="E10" t="s">
-        <v>59</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -874,7 +927,7 @@
         <v>44611</v>
       </c>
       <c r="E11" t="s">
-        <v>61</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -891,7 +944,7 @@
         <v>44611</v>
       </c>
       <c r="E12" t="s">
-        <v>64</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -908,7 +961,7 @@
         <v>44611</v>
       </c>
       <c r="E13" t="s">
-        <v>65</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -925,7 +978,7 @@
         <v>44611</v>
       </c>
       <c r="E14" t="s">
-        <v>65</v>
+        <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -942,7 +995,7 @@
         <v>44611</v>
       </c>
       <c r="E15" t="s">
-        <v>66</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -959,7 +1012,7 @@
         <v>44611</v>
       </c>
       <c r="E16" t="s">
-        <v>63</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -976,7 +1029,7 @@
         <v>44611</v>
       </c>
       <c r="E17" t="s">
-        <v>67</v>
+        <v>112</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -993,7 +1046,7 @@
         <v>44611</v>
       </c>
       <c r="E18" t="s">
-        <v>61</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1010,7 +1063,7 @@
         <v>44611</v>
       </c>
       <c r="E19" t="s">
-        <v>69</v>
+        <v>113</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1027,7 +1080,7 @@
         <v>44611</v>
       </c>
       <c r="E20" t="s">
-        <v>68</v>
+        <v>114</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1044,7 +1097,7 @@
         <v>44611</v>
       </c>
       <c r="E21" t="s">
-        <v>61</v>
+        <v>108</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1061,7 +1114,7 @@
         <v>44611</v>
       </c>
       <c r="E22" t="s">
-        <v>59</v>
+        <v>106</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1078,7 +1131,7 @@
         <v>44611</v>
       </c>
       <c r="E23" t="s">
-        <v>67</v>
+        <v>112</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1095,7 +1148,7 @@
         <v>44611</v>
       </c>
       <c r="E24" t="s">
-        <v>59</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1112,7 +1165,7 @@
         <v>44611</v>
       </c>
       <c r="E25" t="s">
-        <v>61</v>
+        <v>108</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1129,7 +1182,7 @@
         <v>44611</v>
       </c>
       <c r="E26" t="s">
-        <v>70</v>
+        <v>115</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1146,7 +1199,7 @@
         <v>44611</v>
       </c>
       <c r="E27" t="s">
-        <v>69</v>
+        <v>113</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1163,7 +1216,7 @@
         <v>44611</v>
       </c>
       <c r="E28" t="s">
-        <v>59</v>
+        <v>106</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1180,7 +1233,7 @@
         <v>44611</v>
       </c>
       <c r="E29" t="s">
-        <v>35</v>
+        <v>116</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1197,7 +1250,7 @@
         <v>44611</v>
       </c>
       <c r="E30" t="s">
-        <v>59</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1282,7 +1335,7 @@
         <v>44618</v>
       </c>
       <c r="E35" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1316,7 +1369,7 @@
         <v>44618</v>
       </c>
       <c r="E37" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1384,7 +1437,7 @@
         <v>44618</v>
       </c>
       <c r="E41" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1401,7 +1454,7 @@
         <v>44618</v>
       </c>
       <c r="E42" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1412,13 +1465,13 @@
         <v>37</v>
       </c>
       <c r="C43" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D43" s="1">
         <v>44618</v>
       </c>
       <c r="E43" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1497,13 +1550,13 @@
         <v>52</v>
       </c>
       <c r="C48" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D48" s="1">
         <v>44618</v>
       </c>
       <c r="E48" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -1514,13 +1567,13 @@
         <v>52</v>
       </c>
       <c r="C49" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D49" s="1">
         <v>44618</v>
       </c>
       <c r="E49" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1531,7 +1584,7 @@
         <v>52</v>
       </c>
       <c r="C50" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D50" s="1">
         <v>44618</v>
@@ -1554,7 +1607,7 @@
         <v>44618</v>
       </c>
       <c r="E51" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -1582,13 +1635,13 @@
         <v>52</v>
       </c>
       <c r="C53" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D53" s="1">
         <v>44618</v>
       </c>
       <c r="E53" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -1596,16 +1649,16 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C54" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D54" s="1">
         <v>45109</v>
       </c>
       <c r="E54" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -1613,10 +1666,10 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C55" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="D55" s="1">
         <v>45109</v>
@@ -1630,16 +1683,16 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C56" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D56" s="1">
         <v>45109</v>
       </c>
       <c r="E56" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -1647,16 +1700,16 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C57" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D57" s="1">
         <v>45109</v>
       </c>
       <c r="E57" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -1664,10 +1717,10 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C58" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="D58" s="1">
         <v>45109</v>
@@ -1681,10 +1734,10 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C59" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D59" s="1">
         <v>45109</v>
@@ -1698,10 +1751,10 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C60" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D60" s="1">
         <v>45109</v>
@@ -1715,16 +1768,16 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C61" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D61" s="1">
         <v>45109</v>
       </c>
       <c r="E61" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -1732,10 +1785,10 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C62" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D62" s="1">
         <v>45109</v>
@@ -1749,16 +1802,16 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C63" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D63" s="1">
         <v>45109</v>
       </c>
       <c r="E63" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -1766,10 +1819,10 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C64" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D64" s="1">
         <v>45109</v>
@@ -1783,16 +1836,16 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
+        <v>84</v>
+      </c>
+      <c r="C65" t="s">
         <v>90</v>
       </c>
-      <c r="C65" t="s">
-        <v>96</v>
-      </c>
       <c r="D65" s="1">
         <v>45109</v>
       </c>
       <c r="E65" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -1800,10 +1853,10 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C66" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D66" s="1">
         <v>45109</v>
@@ -1817,16 +1870,16 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C67" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D67" s="1">
         <v>45109</v>
       </c>
       <c r="E67" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -1834,16 +1887,16 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C68" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D68" s="1">
         <v>45109</v>
       </c>
       <c r="E68" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -1851,16 +1904,16 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
+        <v>94</v>
+      </c>
+      <c r="C69" t="s">
         <v>100</v>
       </c>
-      <c r="C69" t="s">
-        <v>106</v>
-      </c>
       <c r="D69" s="1">
         <v>45109</v>
       </c>
       <c r="E69" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -1868,10 +1921,10 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C70" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D70" s="1">
         <v>45109</v>
@@ -1885,16 +1938,16 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C71" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D71" s="1">
         <v>45109</v>
       </c>
       <c r="E71" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -1902,16 +1955,16 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C72" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D72" s="1">
         <v>45109</v>
       </c>
       <c r="E72" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -1919,16 +1972,16 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C73" t="s">
+        <v>97</v>
+      </c>
+      <c r="D73" s="1">
+        <v>45109</v>
+      </c>
+      <c r="E73" t="s">
         <v>103</v>
-      </c>
-      <c r="D73" s="1">
-        <v>45109</v>
-      </c>
-      <c r="E73" t="s">
-        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1938,18 +1991,1368 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2134E77E-EC53-4558-98B1-8DF1BED85095}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96EBF91B-2201-4A3A-BD04-CC64612EBAD0}">
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E2"/>
+      <selection sqref="A1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.5703125" customWidth="1"/>
+    <col min="3" max="3" width="255.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" s="1">
+        <v>45109</v>
+      </c>
+      <c r="E2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>54</v>
+      </c>
+      <c r="B3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D3" s="1">
+        <v>45109</v>
+      </c>
+      <c r="E3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>55</v>
+      </c>
+      <c r="B4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" s="1">
+        <v>45109</v>
+      </c>
+      <c r="E4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>56</v>
+      </c>
+      <c r="B5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="1">
+        <v>45109</v>
+      </c>
+      <c r="E5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>57</v>
+      </c>
+      <c r="B6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" s="1">
+        <v>45109</v>
+      </c>
+      <c r="E6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>58</v>
+      </c>
+      <c r="B7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" s="1">
+        <v>45109</v>
+      </c>
+      <c r="E7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>59</v>
+      </c>
+      <c r="B8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8" s="1">
+        <v>45109</v>
+      </c>
+      <c r="E8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>60</v>
+      </c>
+      <c r="B9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D9" s="1">
+        <v>45109</v>
+      </c>
+      <c r="E9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>61</v>
+      </c>
+      <c r="B10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" t="s">
+        <v>87</v>
+      </c>
+      <c r="D10" s="1">
+        <v>45109</v>
+      </c>
+      <c r="E10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>62</v>
+      </c>
+      <c r="B11" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D11" s="1">
+        <v>45109</v>
+      </c>
+      <c r="E11" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>63</v>
+      </c>
+      <c r="B12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" t="s">
+        <v>89</v>
+      </c>
+      <c r="D12" s="1">
+        <v>45109</v>
+      </c>
+      <c r="E12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>64</v>
+      </c>
+      <c r="B13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D13" s="1">
+        <v>45109</v>
+      </c>
+      <c r="E13" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>65</v>
+      </c>
+      <c r="B14" t="s">
+        <v>84</v>
+      </c>
+      <c r="C14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D14" s="1">
+        <v>45109</v>
+      </c>
+      <c r="E14" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>66</v>
+      </c>
+      <c r="B15" t="s">
+        <v>84</v>
+      </c>
+      <c r="C15" t="s">
+        <v>92</v>
+      </c>
+      <c r="D15" s="1">
+        <v>45109</v>
+      </c>
+      <c r="E15" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>67</v>
+      </c>
+      <c r="B16" t="s">
+        <v>84</v>
+      </c>
+      <c r="C16" t="s">
+        <v>93</v>
+      </c>
+      <c r="D16" s="1">
+        <v>45109</v>
+      </c>
+      <c r="E16" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>68</v>
+      </c>
+      <c r="B17" t="s">
+        <v>94</v>
+      </c>
+      <c r="C17" t="s">
+        <v>100</v>
+      </c>
+      <c r="D17" s="1">
+        <v>45109</v>
+      </c>
+      <c r="E17" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>69</v>
+      </c>
+      <c r="B18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D18" s="1">
+        <v>45109</v>
+      </c>
+      <c r="E18" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>70</v>
+      </c>
+      <c r="B19" t="s">
+        <v>94</v>
+      </c>
+      <c r="C19" t="s">
+        <v>96</v>
+      </c>
+      <c r="D19" s="1">
+        <v>45109</v>
+      </c>
+      <c r="E19" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>71</v>
+      </c>
+      <c r="B20" t="s">
+        <v>94</v>
+      </c>
+      <c r="C20" t="s">
+        <v>99</v>
+      </c>
+      <c r="D20" s="1">
+        <v>45109</v>
+      </c>
+      <c r="E20" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>72</v>
+      </c>
+      <c r="B21" t="s">
+        <v>94</v>
+      </c>
+      <c r="C21" t="s">
+        <v>97</v>
+      </c>
+      <c r="D21" s="1">
+        <v>45109</v>
+      </c>
+      <c r="E21" t="s">
+        <v>126</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2134E77E-EC53-4558-98B1-8DF1BED85095}">
+  <dimension ref="A1:E30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="45.42578125" bestFit="1" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" s="1">
+        <v>44611</v>
+      </c>
+      <c r="E2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" s="1">
+        <v>44611</v>
+      </c>
+      <c r="E3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" s="1">
+        <v>44611</v>
+      </c>
+      <c r="E4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" s="1">
+        <v>44611</v>
+      </c>
+      <c r="E5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="1">
+        <v>44611</v>
+      </c>
+      <c r="E6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="1">
+        <v>44611</v>
+      </c>
+      <c r="E7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="1">
+        <v>44611</v>
+      </c>
+      <c r="E8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="1">
+        <v>44611</v>
+      </c>
+      <c r="E9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="1">
+        <v>44611</v>
+      </c>
+      <c r="E10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="1">
+        <v>44611</v>
+      </c>
+      <c r="E11" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="1">
+        <v>44611</v>
+      </c>
+      <c r="E12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="1">
+        <v>44611</v>
+      </c>
+      <c r="E13" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="1">
+        <v>44611</v>
+      </c>
+      <c r="E14" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="1">
+        <v>44611</v>
+      </c>
+      <c r="E15" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="1">
+        <v>44611</v>
+      </c>
+      <c r="E16" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="1">
+        <v>44611</v>
+      </c>
+      <c r="E17" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="1">
+        <v>44611</v>
+      </c>
+      <c r="E18" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="1">
+        <v>44611</v>
+      </c>
+      <c r="E19" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="1">
+        <v>44611</v>
+      </c>
+      <c r="E20" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="1">
+        <v>44611</v>
+      </c>
+      <c r="E21" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="1">
+        <v>44611</v>
+      </c>
+      <c r="E22" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="1">
+        <v>44611</v>
+      </c>
+      <c r="E23" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="1">
+        <v>44611</v>
+      </c>
+      <c r="E24" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="1">
+        <v>44611</v>
+      </c>
+      <c r="E25" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="1">
+        <v>44611</v>
+      </c>
+      <c r="E26" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" s="1">
+        <v>44611</v>
+      </c>
+      <c r="E27" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" s="1">
+        <v>44611</v>
+      </c>
+      <c r="E28" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" t="s">
+        <v>34</v>
+      </c>
+      <c r="D29" s="1">
+        <v>44611</v>
+      </c>
+      <c r="E29" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" t="s">
+        <v>36</v>
+      </c>
+      <c r="D30" s="1">
+        <v>44611</v>
+      </c>
+      <c r="E30" t="s">
+        <v>106</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85D129F9-F35B-4C15-9944-7BF674109462}">
+  <dimension ref="A1:E26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="69.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="1">
+        <v>44618</v>
+      </c>
+      <c r="E2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="1">
+        <v>44618</v>
+      </c>
+      <c r="E3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="1">
+        <v>44618</v>
+      </c>
+      <c r="E4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>33</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="1">
+        <v>44618</v>
+      </c>
+      <c r="E5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="1">
+        <v>44618</v>
+      </c>
+      <c r="E6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="1">
+        <v>44618</v>
+      </c>
+      <c r="E7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>36</v>
+      </c>
+      <c r="B8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="1">
+        <v>44618</v>
+      </c>
+      <c r="E8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>37</v>
+      </c>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="1">
+        <v>44618</v>
+      </c>
+      <c r="E9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>38</v>
+      </c>
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="1">
+        <v>44618</v>
+      </c>
+      <c r="E10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>39</v>
+      </c>
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="1">
+        <v>44618</v>
+      </c>
+      <c r="E11" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>40</v>
+      </c>
+      <c r="B12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="1">
+        <v>44618</v>
+      </c>
+      <c r="E12" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="1">
+        <v>44618</v>
+      </c>
+      <c r="E13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>42</v>
+      </c>
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D14" s="1">
+        <v>44618</v>
+      </c>
+      <c r="E14" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>43</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="1">
+        <v>44618</v>
+      </c>
+      <c r="E15" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>44</v>
+      </c>
+      <c r="B16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="1">
+        <v>44618</v>
+      </c>
+      <c r="E16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>45</v>
+      </c>
+      <c r="B17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" s="1">
+        <v>44618</v>
+      </c>
+      <c r="E17" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>46</v>
+      </c>
+      <c r="B18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" s="1">
+        <v>44618</v>
+      </c>
+      <c r="E18" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>47</v>
+      </c>
+      <c r="B19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" s="1">
+        <v>44618</v>
+      </c>
+      <c r="E19" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>48</v>
+      </c>
+      <c r="B20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" s="1">
+        <v>44618</v>
+      </c>
+      <c r="E20" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>49</v>
+      </c>
+      <c r="B21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" t="s">
+        <v>71</v>
+      </c>
+      <c r="D21" s="1">
+        <v>44618</v>
+      </c>
+      <c r="E21" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>50</v>
+      </c>
+      <c r="B22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" s="1">
+        <v>44618</v>
+      </c>
+      <c r="E22" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>51</v>
+      </c>
+      <c r="B23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="1">
+        <v>44618</v>
+      </c>
+      <c r="E23" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>52</v>
+      </c>
+      <c r="B24" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" t="s">
+        <v>72</v>
+      </c>
+      <c r="D24" s="1">
+        <v>44618</v>
+      </c>
+      <c r="E24" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>53</v>
+      </c>
+      <c r="B25" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" t="s">
+        <v>122</v>
+      </c>
+      <c r="D25" s="1">
+        <v>44983</v>
+      </c>
+      <c r="E25" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>54</v>
+      </c>
+      <c r="B26" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" t="s">
+        <v>123</v>
+      </c>
+      <c r="D26" s="1">
+        <v>44983</v>
+      </c>
+      <c r="E26" t="s">
+        <v>124</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>